<commit_message>
5.5 passed and 4.1 files added
</commit_message>
<xml_diff>
--- a/5sem/55/tables/data_f.xlsx
+++ b/5sem/55/tables/data_f.xlsx
@@ -375,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,7 +730,7 @@
         <v>196.71356655659284</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9" si="10">C9/(1+2*C9/511)</f>
+        <f t="shared" ref="I9:I10" si="10">C9/(1+2*C9/511)</f>
         <v>146.45819394340717</v>
       </c>
       <c r="J9">
@@ -740,6 +740,13 @@
       <c r="K9">
         <f t="shared" si="6"/>
         <v>0.89205570639481535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>